<commit_message>
adding excel chart changes
</commit_message>
<xml_diff>
--- a/ExcelCharts.xlsx
+++ b/ExcelCharts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t xml:space="preserve">Dimensions </t>
   </si>
@@ -37,6 +37,24 @@
   </si>
   <si>
     <t>Running without specifying OMP_NUM_THREADS 10000 Data Points</t>
+  </si>
+  <si>
+    <t>Running without specifying various threads and Data Points</t>
+  </si>
+  <si>
+    <t>Threads</t>
+  </si>
+  <si>
+    <t>Data Points</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Max. Value</t>
   </si>
 </sst>
 </file>
@@ -81,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -113,8 +131,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -122,8 +149,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -134,17 +163,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -325,6 +359,66 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -335,8 +429,8 @@
   <autoFilter ref="B2:D6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Dimensions "/>
-    <tableColumn id="2" name="Matrix Calc Time" dataDxfId="5"/>
-    <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="4"/>
+    <tableColumn id="2" name="Matrix Calc Time" dataDxfId="7"/>
+    <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -347,8 +441,8 @@
   <autoFilter ref="B10:D14"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Dimensions "/>
-    <tableColumn id="2" name="Matrix Calc Time" dataDxfId="3"/>
-    <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="2"/>
+    <tableColumn id="2" name="Matrix Calc Time" dataDxfId="5"/>
+    <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -359,6 +453,22 @@
   <autoFilter ref="B18:D22"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Dimensions "/>
+    <tableColumn id="2" name="Matrix Calc Time" dataDxfId="3"/>
+    <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table145" displayName="Table145" ref="B25:H33" totalsRowShown="0">
+  <autoFilter ref="B25:H33"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Threads"/>
+    <tableColumn id="4" name="Data Points"/>
+    <tableColumn id="5" name="Dimensions"/>
+    <tableColumn id="6" name="K"/>
+    <tableColumn id="7" name="Max. Value"/>
     <tableColumn id="2" name="Matrix Calc Time" dataDxfId="1"/>
     <tableColumn id="3" name="Avg. Seeking Time" dataDxfId="0"/>
   </tableColumns>
@@ -688,17 +798,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D22"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
@@ -821,12 +934,12 @@
         <v>1.12E-4</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:8">
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:8">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -837,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="16" thickBot="1">
+    <row r="19" spans="2:8" ht="16" thickBot="1">
       <c r="B19">
         <v>100</v>
       </c>
@@ -848,7 +961,7 @@
         <v>1.8420000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="16" thickBot="1">
+    <row r="20" spans="2:8" ht="16" thickBot="1">
       <c r="B20">
         <v>1000</v>
       </c>
@@ -859,27 +972,214 @@
         <v>1.534E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="16" thickBot="1">
+    <row r="21" spans="2:8" ht="16" thickBot="1">
       <c r="B21">
         <v>10000</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="16" thickBot="1">
+    <row r="22" spans="2:8" ht="16" thickBot="1">
       <c r="B22">
         <v>100000</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="16" thickBot="1">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>10000</v>
+      </c>
+      <c r="D26">
+        <v>1000</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <v>1000</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="2:8" ht="16" thickBot="1">
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>10000</v>
+      </c>
+      <c r="D27">
+        <v>1000</v>
+      </c>
+      <c r="E27">
+        <v>50</v>
+      </c>
+      <c r="F27">
+        <v>1000</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="2:8" ht="16" thickBot="1">
+      <c r="B28">
+        <f>B27*2</f>
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>10000</v>
+      </c>
+      <c r="D28">
+        <v>1000</v>
+      </c>
+      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <v>1000</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="2:8" ht="16" thickBot="1">
+      <c r="B29">
+        <f t="shared" ref="B29:B33" si="0">B28*2</f>
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>10000</v>
+      </c>
+      <c r="D29">
+        <v>1000</v>
+      </c>
+      <c r="E29">
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <v>1000</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>10000</v>
+      </c>
+      <c r="D30">
+        <v>1000</v>
+      </c>
+      <c r="E30">
+        <v>50</v>
+      </c>
+      <c r="F30">
+        <v>1000</v>
+      </c>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>10000</v>
+      </c>
+      <c r="D31">
+        <v>1000</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="F31">
+        <v>1000</v>
+      </c>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>10000</v>
+      </c>
+      <c r="D32">
+        <v>1000</v>
+      </c>
+      <c r="E32">
+        <v>50</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="C33">
+        <v>10000</v>
+      </c>
+      <c r="D33">
+        <v>1000</v>
+      </c>
+      <c r="E33">
+        <v>50</v>
+      </c>
+      <c r="F33">
+        <v>1000</v>
+      </c>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>